<commit_message>
i am commiting executed code for registration and latestcode
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="17976" windowHeight="8004"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14790" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>key</t>
   </si>
@@ -70,9 +70,6 @@
     <t>(//input[@type='checkbox'])[3]</t>
   </si>
   <si>
-    <t>abc@123456</t>
-  </si>
-  <si>
     <t>//input[@name='passwd2']</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>//input[@name='name']</t>
   </si>
   <si>
-    <t>rashikanna@gmail.com</t>
-  </si>
-  <si>
     <t>//input[@id='email']</t>
   </si>
   <si>
@@ -245,6 +239,18 @@
   </si>
   <si>
     <t>(//table)[9]//tr/td/a</t>
+  </si>
+  <si>
+    <t>asdfgh@gmail.com</t>
+  </si>
+  <si>
+    <t>abc12345</t>
+  </si>
+  <si>
+    <t>D:\Eclipse-1.1\pageobject model\ColourClassifieds\TestData.xlsx</t>
+  </si>
+  <si>
+    <t>excel_filepath</t>
   </si>
 </sst>
 </file>
@@ -297,13 +303,16 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -599,16 +608,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.21875" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -624,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -632,7 +641,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -640,7 +649,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -648,15 +657,15 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -664,7 +673,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -672,7 +681,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -680,7 +689,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -688,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -696,15 +705,15 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
+      <c r="B12" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -725,215 +734,226 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" customFormat="1" ht="45">
+      <c r="A21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" customFormat="1"/>
+    <row r="23" spans="1:2" customFormat="1">
+      <c r="A23" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" customFormat="1">
+      <c r="A24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="5" t="s">
+    <row r="25" spans="1:2" customFormat="1">
+      <c r="A25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" customFormat="1">
+      <c r="A26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" customFormat="1">
+      <c r="A27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
+    <row r="28" spans="1:2" customFormat="1">
+      <c r="A28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" customFormat="1">
+      <c r="A29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
         <v>43</v>
       </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="30" spans="1:2" customFormat="1">
+      <c r="A30" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
+      <c r="B30" t="s">
         <v>50</v>
       </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
+    </row>
+    <row r="31" spans="1:2" customFormat="1">
+      <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" customFormat="1">
+      <c r="A32" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="2" t="s">
+      <c r="B32" t="s">
         <v>53</v>
       </c>
-      <c r="B30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="33" spans="1:2" customFormat="1">
+      <c r="A33" s="2" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>62</v>
       </c>
       <c r="B33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="2" t="s">
+    <row r="34" spans="1:2" customFormat="1">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" customFormat="1">
+      <c r="A36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" customFormat="1">
+      <c r="A37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" customFormat="1">
+      <c r="A39" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" customFormat="1">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" customFormat="1">
+      <c r="A41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" customFormat="1">
+      <c r="A42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" customFormat="1">
+      <c r="A44" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" customFormat="1">
+      <c r="A45" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="1" t="s">
+      <c r="B45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+    <row r="46" spans="1:2" customFormat="1">
+      <c r="A46" t="s">
         <v>72</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId1" display="abc@12345"/>
     <hyperlink ref="B15" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B12" r:id="rId4" display="abc@12345"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -943,7 +963,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -955,7 +975,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>